<commit_message>
System1 login sequence - initial actions
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karolina_Mamczarz\Desktop\RPA\Calculate_Client_Security_Hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685C8A91-DCFC-4BDE-B9F1-E632F05E26CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E158243-397F-4B94-B27F-B33D0F6A4ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -545,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1629,7 +1629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>